<commit_message>
add: phase 3 report
</commit_message>
<xml_diff>
--- a/Phase 3 - Language Definition/Language resource template.xlsx
+++ b/Phase 3 - Language Definition/Language resource template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e28296c225434f2/Documents/2024 spring/kge/Transportation-Facilities-KGE-Project/Phase 3 - Language Definition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_8028100C632B1C21BA12AF74CEB588236EC4F7EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{266C3C10-3FA3-4F44-9FEA-C797795D4D8D}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_8028100C632B1C21BA12AF74CEB588236EC4F7EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD746CF-FA7B-4225-829A-87600A15EAD8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
-    <t>ConcetID</t>
-  </si>
-  <si>
     <t>Word-en</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Тээврийн (завь, автобус, машин, онгоц, галт тэрэг зэрэг) хэрэгслийг жолоодохгүйгээр сууж байгаа аялагч.</t>
+  </si>
+  <si>
+    <t>ConceptID</t>
   </si>
 </sst>
 </file>
@@ -246,6 +246,14 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -449,8 +457,8 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -464,104 +472,104 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>